<commit_message>
Removing the duplicate rows handler since we now have a Unique Identifier made of Link ID and SLA ID
</commit_message>
<xml_diff>
--- a/Data/LTK SLA & Invoice.xlsx
+++ b/Data/LTK SLA & Invoice.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6019e03d3618181c/KRA WORK/2024 WS/SLA EDA/SLA_ETL/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{4CE40AE1-F42C-4691-AA0D-27D04A5C7DEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C31143C-600C-4A48-88EB-66F77BF13A00}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{4CE40AE1-F42C-4691-AA0D-27D04A5C7DEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E6852D3-3EAF-49E7-B842-B243FBDB5EF4}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E3BAD0CB-983C-4598-BC59-C1CADFA80182}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{E3BAD0CB-983C-4598-BC59-C1CADFA80182}"/>
   </bookViews>
   <sheets>
     <sheet name="SLA" sheetId="1" r:id="rId1"/>
@@ -1032,6 +1032,10 @@
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
+<file path=xl/persons/person0.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2BCBDC4E-C1EE-4678-AA72-447EA4D993DF}" name="Table1" displayName="Table1" ref="A1:K27" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21" headerRowCellStyle="Normal 2">
   <autoFilter ref="A1:K27" xr:uid="{2BCBDC4E-C1EE-4678-AA72-447EA4D993DF}"/>
@@ -1057,6 +1061,9 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5F18262D-995C-449D-BBAF-58D72757A9AE}" name="Table13" displayName="Table13" ref="A1:I27" totalsRowShown="0" dataDxfId="9" headerRowCellStyle="Normal 2" dataCellStyle="Comma 2">
   <autoFilter ref="A1:I27" xr:uid="{5F18262D-995C-449D-BBAF-58D72757A9AE}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I27">
+    <sortCondition descending="1" ref="D2:D27"/>
+  </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{D4D352A5-4D04-4B6B-9983-C880F5EDB338}" name="Invoice Date" dataDxfId="8" dataCellStyle="Normal 2"/>
     <tableColumn id="2" xr3:uid="{B112AAB4-CDB8-41C2-A54B-B3FC565D6611}" name="Invoice No" dataDxfId="7" dataCellStyle="Normal 2"/>
@@ -1378,8 +1385,8 @@
   </sheetPr>
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="C13" zoomScale="77" zoomScaleNormal="70" zoomScaleSheetLayoutView="77" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView view="pageBreakPreview" zoomScale="77" zoomScaleNormal="70" zoomScaleSheetLayoutView="77" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2379,16 +2386,16 @@
   </sheetPr>
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="E1" zoomScale="106" zoomScaleNormal="100" zoomScaleSheetLayoutView="106" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="106" zoomScaleNormal="100" zoomScaleSheetLayoutView="106" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.42578125" customWidth="1"/>
+    <col min="4" max="4" width="29.28515625" customWidth="1"/>
     <col min="5" max="5" width="74.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -2427,33 +2434,33 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="29">
-        <v>45212</v>
-      </c>
-      <c r="B2" s="28" t="s">
-        <v>84</v>
+        <v>45205</v>
+      </c>
+      <c r="B2" s="30">
+        <v>116426</v>
       </c>
       <c r="C2" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="D2" s="30">
-        <v>26046</v>
+      <c r="D2" s="30" t="s">
+        <v>113</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>86</v>
+        <v>114</v>
       </c>
       <c r="F2" s="31">
-        <v>-48264</v>
+        <v>539154</v>
       </c>
       <c r="G2" s="31">
         <v>0</v>
       </c>
       <c r="H2" s="31">
         <f>0.16*(SUM(Table13[[#This Row],[QRC (EX TAX)]:[Excise (15%)]]))</f>
-        <v>-7722.24</v>
+        <v>86264.639999999999</v>
       </c>
       <c r="I2" s="31">
         <f>SUM(Table13[[#This Row],[QRC (EX TAX)]:[VAT (16%)]])</f>
-        <v>-55986.239999999998</v>
+        <v>625418.64</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2467,24 +2474,24 @@
         <v>85</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>73</v>
+        <v>115</v>
       </c>
       <c r="E3" s="28" t="s">
-        <v>87</v>
-      </c>
-      <c r="F3" s="31">
-        <v>360000</v>
+        <v>116</v>
+      </c>
+      <c r="F3" s="33">
+        <v>96528</v>
       </c>
       <c r="G3" s="31">
         <v>0</v>
       </c>
       <c r="H3" s="31">
         <f>0.16*(SUM(Table13[[#This Row],[QRC (EX TAX)]:[Excise (15%)]]))</f>
-        <v>57600</v>
+        <v>15444.48</v>
       </c>
       <c r="I3" s="31">
         <f>SUM(Table13[[#This Row],[QRC (EX TAX)]:[VAT (16%)]])</f>
-        <v>417600</v>
+        <v>111972.48</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -2497,25 +2504,25 @@
       <c r="C4" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="D4" s="32">
-        <v>1750</v>
+      <c r="D4" s="30" t="s">
+        <v>109</v>
       </c>
       <c r="E4" s="28" t="s">
-        <v>88</v>
+        <v>110</v>
       </c>
       <c r="F4" s="33">
-        <v>810000</v>
+        <v>120000</v>
       </c>
       <c r="G4" s="31">
         <v>0</v>
       </c>
       <c r="H4" s="31">
         <f>0.16*(SUM(Table13[[#This Row],[QRC (EX TAX)]:[Excise (15%)]]))</f>
-        <v>129600</v>
+        <v>19200</v>
       </c>
       <c r="I4" s="31">
         <f>SUM(Table13[[#This Row],[QRC (EX TAX)]:[VAT (16%)]])</f>
-        <v>939600</v>
+        <v>139200</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -2528,25 +2535,25 @@
       <c r="C5" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="D5" s="32">
-        <v>5611</v>
+      <c r="D5" s="30" t="s">
+        <v>79</v>
       </c>
       <c r="E5" s="28" t="s">
-        <v>89</v>
-      </c>
-      <c r="F5" s="31">
-        <v>61927.5</v>
+        <v>108</v>
+      </c>
+      <c r="F5" s="33">
+        <v>57002.85</v>
       </c>
       <c r="G5" s="31">
         <v>0</v>
       </c>
       <c r="H5" s="31">
         <f>0.16*(SUM(Table13[[#This Row],[QRC (EX TAX)]:[Excise (15%)]]))</f>
-        <v>9908.4</v>
+        <v>9120.4560000000001</v>
       </c>
       <c r="I5" s="31">
         <f>SUM(Table13[[#This Row],[QRC (EX TAX)]:[VAT (16%)]])</f>
-        <v>71835.899999999994</v>
+        <v>66123.305999999997</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -2559,25 +2566,25 @@
       <c r="C6" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="D6" s="30">
-        <v>20103</v>
+      <c r="D6" s="30" t="s">
+        <v>76</v>
       </c>
       <c r="E6" s="28" t="s">
-        <v>90</v>
-      </c>
-      <c r="F6" s="31">
-        <v>68850</v>
+        <v>107</v>
+      </c>
+      <c r="F6" s="33">
+        <v>96528</v>
       </c>
       <c r="G6" s="31">
         <v>0</v>
       </c>
       <c r="H6" s="31">
         <f>0.16*(SUM(Table13[[#This Row],[QRC (EX TAX)]:[Excise (15%)]]))</f>
-        <v>11016</v>
+        <v>15444.48</v>
       </c>
       <c r="I6" s="31">
         <f>SUM(Table13[[#This Row],[QRC (EX TAX)]:[VAT (16%)]])</f>
-        <v>79866</v>
+        <v>111972.48</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -2590,25 +2597,25 @@
       <c r="C7" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="D7" s="30">
-        <v>20954</v>
+      <c r="D7" s="30" t="s">
+        <v>105</v>
       </c>
       <c r="E7" s="28" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="F7" s="33">
-        <v>150000</v>
+        <v>57000</v>
       </c>
       <c r="G7" s="31">
         <v>0</v>
       </c>
       <c r="H7" s="31">
         <f>0.16*(SUM(Table13[[#This Row],[QRC (EX TAX)]:[Excise (15%)]]))</f>
-        <v>24000</v>
+        <v>9120</v>
       </c>
       <c r="I7" s="31">
         <f>SUM(Table13[[#This Row],[QRC (EX TAX)]:[VAT (16%)]])</f>
-        <v>174000</v>
+        <v>66120</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -2621,25 +2628,25 @@
       <c r="C8" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="D8" s="30">
-        <v>21195</v>
+      <c r="D8" s="30" t="s">
+        <v>101</v>
       </c>
       <c r="E8" s="28" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="F8" s="33">
-        <v>432000</v>
+        <v>96528</v>
       </c>
       <c r="G8" s="31">
         <v>0</v>
       </c>
       <c r="H8" s="31">
         <f>0.16*(SUM(Table13[[#This Row],[QRC (EX TAX)]:[Excise (15%)]]))</f>
-        <v>69120</v>
+        <v>15444.48</v>
       </c>
       <c r="I8" s="31">
         <f>SUM(Table13[[#This Row],[QRC (EX TAX)]:[VAT (16%)]])</f>
-        <v>501120</v>
+        <v>111972.48</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -2652,25 +2659,25 @@
       <c r="C9" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="D9" s="30">
-        <v>23945</v>
+      <c r="D9" s="30" t="s">
+        <v>111</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>93</v>
+        <v>112</v>
       </c>
       <c r="F9" s="33">
-        <v>60000</v>
+        <v>360000</v>
       </c>
       <c r="G9" s="31">
         <v>0</v>
       </c>
       <c r="H9" s="31">
         <f>0.16*(SUM(Table13[[#This Row],[QRC (EX TAX)]:[Excise (15%)]]))</f>
-        <v>9600</v>
+        <v>57600</v>
       </c>
       <c r="I9" s="31">
         <f>SUM(Table13[[#This Row],[QRC (EX TAX)]:[VAT (16%)]])</f>
-        <v>69600</v>
+        <v>417600</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -2683,25 +2690,25 @@
       <c r="C10" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="D10" s="34">
-        <v>24174</v>
-      </c>
-      <c r="E10" s="35" t="s">
-        <v>94</v>
+      <c r="D10" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" s="28" t="s">
+        <v>103</v>
       </c>
       <c r="F10" s="31">
-        <v>57000</v>
+        <v>1080000</v>
       </c>
       <c r="G10" s="31">
-        <v>0</v>
+        <v>162000</v>
       </c>
       <c r="H10" s="31">
         <f>0.16*(SUM(Table13[[#This Row],[QRC (EX TAX)]:[Excise (15%)]]))</f>
-        <v>9120</v>
+        <v>198720</v>
       </c>
       <c r="I10" s="31">
         <f>SUM(Table13[[#This Row],[QRC (EX TAX)]:[VAT (16%)]])</f>
-        <v>66120</v>
+        <v>1440720</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -2714,25 +2721,25 @@
       <c r="C11" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="D11" s="30">
-        <v>25102</v>
+      <c r="D11" s="30" t="s">
+        <v>69</v>
       </c>
       <c r="E11" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="F11" s="33">
-        <v>162000</v>
+        <v>104</v>
+      </c>
+      <c r="F11" s="31">
+        <v>810000</v>
       </c>
       <c r="G11" s="31">
         <v>0</v>
       </c>
       <c r="H11" s="31">
         <f>0.16*(SUM(Table13[[#This Row],[QRC (EX TAX)]:[Excise (15%)]]))</f>
-        <v>25920</v>
+        <v>129600</v>
       </c>
       <c r="I11" s="31">
         <f>SUM(Table13[[#This Row],[QRC (EX TAX)]:[VAT (16%)]])</f>
-        <v>187920</v>
+        <v>939600</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -2745,25 +2752,25 @@
       <c r="C12" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="D12" s="30">
-        <v>25106</v>
+      <c r="D12" s="30" t="s">
+        <v>97</v>
       </c>
       <c r="E12" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="F12" s="31">
-        <v>57000</v>
+        <v>98</v>
+      </c>
+      <c r="F12" s="33">
+        <v>120000</v>
       </c>
       <c r="G12" s="31">
         <v>0</v>
       </c>
       <c r="H12" s="31">
         <f>0.16*(SUM(Table13[[#This Row],[QRC (EX TAX)]:[Excise (15%)]]))</f>
-        <v>9120</v>
+        <v>19200</v>
       </c>
       <c r="I12" s="31">
         <f>SUM(Table13[[#This Row],[QRC (EX TAX)]:[VAT (16%)]])</f>
-        <v>66120</v>
+        <v>139200</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -2776,25 +2783,25 @@
       <c r="C13" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="D13" s="30">
-        <v>26046</v>
+      <c r="D13" s="30" t="s">
+        <v>73</v>
       </c>
       <c r="E13" s="28" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F13" s="31">
-        <v>48264</v>
+        <v>360000</v>
       </c>
       <c r="G13" s="31">
         <v>0</v>
       </c>
       <c r="H13" s="31">
         <f>0.16*(SUM(Table13[[#This Row],[QRC (EX TAX)]:[Excise (15%)]]))</f>
-        <v>7722.24</v>
+        <v>57600</v>
       </c>
       <c r="I13" s="31">
         <f>SUM(Table13[[#This Row],[QRC (EX TAX)]:[VAT (16%)]])</f>
-        <v>55986.239999999998</v>
+        <v>417600</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -2808,24 +2815,24 @@
         <v>85</v>
       </c>
       <c r="D14" s="30" t="s">
-        <v>97</v>
+        <v>119</v>
       </c>
       <c r="E14" s="28" t="s">
-        <v>98</v>
-      </c>
-      <c r="F14" s="33">
-        <v>120000</v>
+        <v>120</v>
+      </c>
+      <c r="F14" s="31">
+        <v>48000</v>
       </c>
       <c r="G14" s="31">
         <v>0</v>
       </c>
       <c r="H14" s="31">
         <f>0.16*(SUM(Table13[[#This Row],[QRC (EX TAX)]:[Excise (15%)]]))</f>
-        <v>19200</v>
+        <v>7680</v>
       </c>
       <c r="I14" s="31">
         <f>SUM(Table13[[#This Row],[QRC (EX TAX)]:[VAT (16%)]])</f>
-        <v>139200</v>
+        <v>55680</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -2839,24 +2846,24 @@
         <v>85</v>
       </c>
       <c r="D15" s="30" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
       <c r="E15" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="F15" s="33">
-        <v>120000</v>
+        <v>118</v>
+      </c>
+      <c r="F15" s="31">
+        <v>28500</v>
       </c>
       <c r="G15" s="31">
         <v>0</v>
       </c>
       <c r="H15" s="31">
         <f>0.16*(SUM(Table13[[#This Row],[QRC (EX TAX)]:[Excise (15%)]]))</f>
-        <v>19200</v>
+        <v>4560</v>
       </c>
       <c r="I15" s="31">
         <f>SUM(Table13[[#This Row],[QRC (EX TAX)]:[VAT (16%)]])</f>
-        <v>139200</v>
+        <v>33060</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -2870,24 +2877,24 @@
         <v>85</v>
       </c>
       <c r="D16" s="30" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E16" s="28" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F16" s="33">
-        <v>96528</v>
+        <v>120000</v>
       </c>
       <c r="G16" s="31">
         <v>0</v>
       </c>
       <c r="H16" s="31">
         <f>0.16*(SUM(Table13[[#This Row],[QRC (EX TAX)]:[Excise (15%)]]))</f>
-        <v>15444.48</v>
+        <v>19200</v>
       </c>
       <c r="I16" s="31">
         <f>SUM(Table13[[#This Row],[QRC (EX TAX)]:[VAT (16%)]])</f>
-        <v>111972.48</v>
+        <v>139200</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -2900,56 +2907,56 @@
       <c r="C17" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="D17" s="30" t="s">
-        <v>65</v>
+      <c r="D17" s="30">
+        <v>26046</v>
       </c>
       <c r="E17" s="28" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="F17" s="31">
-        <v>1080000</v>
+        <v>48264</v>
       </c>
       <c r="G17" s="31">
-        <v>162000</v>
+        <v>0</v>
       </c>
       <c r="H17" s="31">
         <f>0.16*(SUM(Table13[[#This Row],[QRC (EX TAX)]:[Excise (15%)]]))</f>
-        <v>198720</v>
+        <v>7722.24</v>
       </c>
       <c r="I17" s="31">
         <f>SUM(Table13[[#This Row],[QRC (EX TAX)]:[VAT (16%)]])</f>
-        <v>1440720</v>
+        <v>55986.239999999998</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="29">
-        <v>45205</v>
-      </c>
-      <c r="B18" s="30">
-        <v>116426</v>
+        <v>45212</v>
+      </c>
+      <c r="B18" s="28" t="s">
+        <v>84</v>
       </c>
       <c r="C18" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="D18" s="30" t="s">
-        <v>69</v>
+      <c r="D18" s="30">
+        <v>26046</v>
       </c>
       <c r="E18" s="28" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="F18" s="31">
-        <v>810000</v>
+        <v>-48264</v>
       </c>
       <c r="G18" s="31">
         <v>0</v>
       </c>
       <c r="H18" s="31">
         <f>0.16*(SUM(Table13[[#This Row],[QRC (EX TAX)]:[Excise (15%)]]))</f>
-        <v>129600</v>
+        <v>-7722.24</v>
       </c>
       <c r="I18" s="31">
         <f>SUM(Table13[[#This Row],[QRC (EX TAX)]:[VAT (16%)]])</f>
-        <v>939600</v>
+        <v>-55986.239999999998</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -2962,13 +2969,13 @@
       <c r="C19" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="D19" s="30" t="s">
-        <v>105</v>
+      <c r="D19" s="30">
+        <v>25106</v>
       </c>
       <c r="E19" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="F19" s="33">
+        <v>96</v>
+      </c>
+      <c r="F19" s="31">
         <v>57000</v>
       </c>
       <c r="G19" s="31">
@@ -2993,25 +3000,25 @@
       <c r="C20" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="D20" s="30" t="s">
-        <v>76</v>
+      <c r="D20" s="30">
+        <v>25102</v>
       </c>
       <c r="E20" s="28" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="F20" s="33">
-        <v>96528</v>
+        <v>162000</v>
       </c>
       <c r="G20" s="31">
         <v>0</v>
       </c>
       <c r="H20" s="31">
         <f>0.16*(SUM(Table13[[#This Row],[QRC (EX TAX)]:[Excise (15%)]]))</f>
-        <v>15444.48</v>
+        <v>25920</v>
       </c>
       <c r="I20" s="31">
         <f>SUM(Table13[[#This Row],[QRC (EX TAX)]:[VAT (16%)]])</f>
-        <v>111972.48</v>
+        <v>187920</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -3024,25 +3031,25 @@
       <c r="C21" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="D21" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="E21" s="28" t="s">
-        <v>108</v>
-      </c>
-      <c r="F21" s="33">
-        <v>57002.85</v>
+      <c r="D21" s="34">
+        <v>24174</v>
+      </c>
+      <c r="E21" s="35" t="s">
+        <v>94</v>
+      </c>
+      <c r="F21" s="31">
+        <v>57000</v>
       </c>
       <c r="G21" s="31">
         <v>0</v>
       </c>
       <c r="H21" s="31">
         <f>0.16*(SUM(Table13[[#This Row],[QRC (EX TAX)]:[Excise (15%)]]))</f>
-        <v>9120.4560000000001</v>
+        <v>9120</v>
       </c>
       <c r="I21" s="31">
         <f>SUM(Table13[[#This Row],[QRC (EX TAX)]:[VAT (16%)]])</f>
-        <v>66123.305999999997</v>
+        <v>66120</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -3055,25 +3062,25 @@
       <c r="C22" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="D22" s="30" t="s">
-        <v>109</v>
+      <c r="D22" s="30">
+        <v>23945</v>
       </c>
       <c r="E22" s="28" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="F22" s="33">
-        <v>120000</v>
+        <v>60000</v>
       </c>
       <c r="G22" s="31">
         <v>0</v>
       </c>
       <c r="H22" s="31">
         <f>0.16*(SUM(Table13[[#This Row],[QRC (EX TAX)]:[Excise (15%)]]))</f>
-        <v>19200</v>
+        <v>9600</v>
       </c>
       <c r="I22" s="31">
         <f>SUM(Table13[[#This Row],[QRC (EX TAX)]:[VAT (16%)]])</f>
-        <v>139200</v>
+        <v>69600</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -3086,25 +3093,25 @@
       <c r="C23" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="D23" s="30" t="s">
-        <v>111</v>
+      <c r="D23" s="30">
+        <v>21195</v>
       </c>
       <c r="E23" s="28" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="F23" s="33">
-        <v>360000</v>
+        <v>432000</v>
       </c>
       <c r="G23" s="31">
         <v>0</v>
       </c>
       <c r="H23" s="31">
         <f>0.16*(SUM(Table13[[#This Row],[QRC (EX TAX)]:[Excise (15%)]]))</f>
-        <v>57600</v>
+        <v>69120</v>
       </c>
       <c r="I23" s="31">
         <f>SUM(Table13[[#This Row],[QRC (EX TAX)]:[VAT (16%)]])</f>
-        <v>417600</v>
+        <v>501120</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -3117,25 +3124,25 @@
       <c r="C24" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="D24" s="30" t="s">
-        <v>113</v>
+      <c r="D24" s="30">
+        <v>20954</v>
       </c>
       <c r="E24" s="28" t="s">
-        <v>114</v>
-      </c>
-      <c r="F24" s="31">
-        <v>539154</v>
+        <v>91</v>
+      </c>
+      <c r="F24" s="33">
+        <v>150000</v>
       </c>
       <c r="G24" s="31">
         <v>0</v>
       </c>
       <c r="H24" s="31">
         <f>0.16*(SUM(Table13[[#This Row],[QRC (EX TAX)]:[Excise (15%)]]))</f>
-        <v>86264.639999999999</v>
+        <v>24000</v>
       </c>
       <c r="I24" s="31">
         <f>SUM(Table13[[#This Row],[QRC (EX TAX)]:[VAT (16%)]])</f>
-        <v>625418.64</v>
+        <v>174000</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -3148,25 +3155,25 @@
       <c r="C25" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="D25" s="30" t="s">
-        <v>115</v>
+      <c r="D25" s="30">
+        <v>20103</v>
       </c>
       <c r="E25" s="28" t="s">
-        <v>116</v>
-      </c>
-      <c r="F25" s="33">
-        <v>96528</v>
+        <v>90</v>
+      </c>
+      <c r="F25" s="31">
+        <v>68850</v>
       </c>
       <c r="G25" s="31">
         <v>0</v>
       </c>
       <c r="H25" s="31">
         <f>0.16*(SUM(Table13[[#This Row],[QRC (EX TAX)]:[Excise (15%)]]))</f>
-        <v>15444.48</v>
+        <v>11016</v>
       </c>
       <c r="I25" s="31">
         <f>SUM(Table13[[#This Row],[QRC (EX TAX)]:[VAT (16%)]])</f>
-        <v>111972.48</v>
+        <v>79866</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -3179,25 +3186,25 @@
       <c r="C26" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="D26" s="30" t="s">
-        <v>117</v>
+      <c r="D26" s="32">
+        <v>5611</v>
       </c>
       <c r="E26" s="28" t="s">
-        <v>118</v>
+        <v>89</v>
       </c>
       <c r="F26" s="31">
-        <v>28500</v>
+        <v>61927.5</v>
       </c>
       <c r="G26" s="31">
         <v>0</v>
       </c>
       <c r="H26" s="31">
         <f>0.16*(SUM(Table13[[#This Row],[QRC (EX TAX)]:[Excise (15%)]]))</f>
-        <v>4560</v>
+        <v>9908.4</v>
       </c>
       <c r="I26" s="31">
         <f>SUM(Table13[[#This Row],[QRC (EX TAX)]:[VAT (16%)]])</f>
-        <v>33060</v>
+        <v>71835.899999999994</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -3210,30 +3217,30 @@
       <c r="C27" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="D27" s="30" t="s">
-        <v>119</v>
+      <c r="D27" s="32">
+        <v>1750</v>
       </c>
       <c r="E27" s="28" t="s">
-        <v>120</v>
-      </c>
-      <c r="F27" s="31">
-        <v>48000</v>
+        <v>88</v>
+      </c>
+      <c r="F27" s="33">
+        <v>810000</v>
       </c>
       <c r="G27" s="31">
         <v>0</v>
       </c>
       <c r="H27" s="31">
         <f>0.16*(SUM(Table13[[#This Row],[QRC (EX TAX)]:[Excise (15%)]]))</f>
-        <v>7680</v>
+        <v>129600</v>
       </c>
       <c r="I27" s="31">
         <f>SUM(Table13[[#This Row],[QRC (EX TAX)]:[VAT (16%)]])</f>
-        <v>55680</v>
+        <v>939600</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="46" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="40" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>